<commit_message>
handling date field from excel, ignoring failures on unknown properties
</commit_message>
<xml_diff>
--- a/excel-connector-impl/src/test/resources/sample.xlsx
+++ b/excel-connector-impl/src/test/resources/sample.xlsx
@@ -5,11 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Sno</t>
   </si>
@@ -32,6 +31,9 @@
     <t xml:space="preserve">Email address</t>
   </si>
   <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">a</t>
   </si>
   <si>
@@ -44,24 +46,34 @@
     <t xml:space="preserve">b@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">c</t>
   </si>
   <si>
     <t xml:space="preserve">c@mail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">1994-11-05T08:15:30-05:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">d</t>
   </si>
   <si>
     <t xml:space="preserve">d@mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1994-11-05T13:15:30Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -136,12 +148,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,15 +182,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,16 +203,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>43551</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -200,13 +226,48 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="c@mail.com"/>
+    <hyperlink ref="C5" r:id="rId2" display="d@mail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -215,68 +276,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="c@mail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="d@mail.com"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>